<commit_message>
Code Merge  - Test Data Files - Companies - 8th Oct 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTI0046461_VerifyCompaniesRelatedListOpportunitiesEngagementEnhancedWithFiltering.xlsx
+++ b/TestData/TMTI0046461_VerifyCompaniesRelatedListOpportunitiesEngagementEnhancedWithFiltering.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VKumar0427\source\repos\SF_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkumar0427\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64B3390-0B55-44AC-8E87-1ACBE0CDD319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4490C645-DA0F-417F-87B5-6C6DEC632F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14640" xr2:uid="{D381DC3E-0C7A-48CF-8E3B-36CB765DCADA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{D381DC3E-0C7A-48CF-8E3B-36CB765DCADA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Companies" sheetId="1" r:id="rId1"/>
-    <sheet name="AppName" sheetId="6" r:id="rId2"/>
-    <sheet name="ModuleName" sheetId="7" r:id="rId3"/>
-    <sheet name="Users" sheetId="2" r:id="rId4"/>
+    <sheet name="Users" sheetId="2" r:id="rId1"/>
+    <sheet name="Companies" sheetId="1" r:id="rId2"/>
+    <sheet name="AppName" sheetId="6" r:id="rId3"/>
+    <sheet name="ModuleName" sheetId="7" r:id="rId4"/>
     <sheet name="TabName" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>StdUser</t>
   </si>
@@ -123,19 +123,31 @@
     <t>Burke Williams, Inc.</t>
   </si>
   <si>
-    <t>Project Chavez</t>
-  </si>
-  <si>
     <t>Project Miura</t>
   </si>
   <si>
     <t>120228</t>
   </si>
   <si>
-    <t>120227</t>
-  </si>
-  <si>
-    <t>Book Prep/Underwriting</t>
+    <t>Burke Williams Eng</t>
+  </si>
+  <si>
+    <t>Burke Williams Spa</t>
+  </si>
+  <si>
+    <t>1459</t>
+  </si>
+  <si>
+    <t>Dead</t>
+  </si>
+  <si>
+    <t>130396</t>
+  </si>
+  <si>
+    <t>133753</t>
+  </si>
+  <si>
+    <t>Retained</t>
   </si>
 </sst>
 </file>
@@ -203,9 +215,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -243,7 +255,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -349,7 +361,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -491,108 +503,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DDA40C-CB43-498D-A2ED-A0851564593B}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A3F6A9-43ED-49B3-9AC1-A223C8D04358}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -601,6 +540,123 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DDA40C-CB43-498D-A2ED-A0851564593B}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6978B76C-41D6-4CB8-BB5A-CE3CBB65EA6D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -608,17 +664,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -628,7 +684,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1988A2C0-E26B-4053-9887-74900EAFFAF5}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -636,49 +692,19 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A3F6A9-43ED-49B3-9AC1-A223C8D04358}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -691,18 +717,18 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -720,7 +746,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -734,7 +760,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -742,13 +768,13 @@
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
     </row>
   </sheetData>

</xml_diff>